<commit_message>
New test added for login also done some cinfig changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91877\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91877\OneDrive\Documents\NovemberBatch\SwagDemo\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1E0093-2B0E-499D-95B2-33C0AC83A6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D8EF8F-354B-4311-AB9E-A24E69A6E250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3664B84B-492A-49DA-A653-E6CE74507088}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3664B84B-492A-49DA-A653-E6CE74507088}"/>
   </bookViews>
   <sheets>
     <sheet name="Creds" sheetId="4" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Subodh</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>standard_user</t>
   </si>
@@ -41,13 +38,25 @@
   </si>
   <si>
     <t>12345</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Data Field</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,18 +65,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,18 +90,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,36 +411,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A336EB-4AE5-45C0-8817-8EBA35377C17}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="Arise@gmail.com" xr:uid="{B1CBC6D1-48D9-41C0-A35E-AD07E209CC0C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -449,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01549EE9-7D09-4ED9-962E-1B5CB201E4ED}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,12 +467,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>